<commit_message>
Update Module 1 template
</commit_message>
<xml_diff>
--- a/public/templates/NHWA_Module_1.xlsx
+++ b/public/templates/NHWA_Module_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20368"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\Final friday\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4748BFA7-9731-48CC-BE11-026CF78DBE3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170F7B5-9FDD-48AD-AA8A-C9295F2817F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ZzPHAP2X1LEhzickjAxTwFeFsu64OF2YSV9noiGGILhhia7PwjhHof1YVZjpCJLGeWi4dVUPnFnvXCPTB91hvA==" workbookSaltValue="Qc1qE8MbNZmsa3u02F1Qfw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -9514,19 +9514,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9928,25 +9928,25 @@
       <c r="A1" s="42" t="s">
         <v>991</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
       <c r="V1" s="12"/>
@@ -9966,25 +9966,25 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="13" t="e">
@@ -10152,41 +10152,41 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47" t="s">
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47" t="s">
+      <c r="I6" s="48"/>
+      <c r="J6" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47" t="s">
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47" t="s">
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48" t="s">
         <v>868</v>
       </c>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
       <c r="Y6" s="8" t="s">
         <v>160</v>
       </c>
@@ -10213,9 +10213,9 @@
       </c>
     </row>
     <row r="7" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="18" t="s">
         <v>45</v>
       </c>
@@ -13461,13 +13461,13 @@
       </c>
     </row>
     <row r="69" spans="2:31" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="47" t="s">
+      <c r="B69" s="48" t="s">
         <v>2626</v>
       </c>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
       <c r="Y69" s="8" t="s">
         <v>116</v>
       </c>
@@ -13494,11 +13494,11 @@
       </c>
     </row>
     <row r="70" spans="2:31" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="50"/>
-      <c r="E70" s="50"/>
-      <c r="F70" s="50"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="49"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="49"/>
       <c r="Y70" s="8" t="s">
         <v>117</v>
       </c>
@@ -18626,6 +18626,11 @@
     <protectedRange sqref="D9:R17 Q4 D19:R23 D25:R67 D8:T8 D18:T18 D24:T24" name="Range1"/>
   </protectedRanges>
   <mergeCells count="12">
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="R6:T6"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="B2:R2"/>
     <mergeCell ref="E6:G6"/>
@@ -18633,11 +18638,6 @@
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="R6:T6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:T67" xr:uid="{AAA47058-289B-4A8A-B387-ECA3D8362AA8}">
@@ -18694,36 +18694,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
       <c r="N2" s="8" t="e">
         <f>Demographic!V2</f>
         <v>#N/A</v>
@@ -18748,7 +18748,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="31">
-        <f>Demographic!V1</f>
+        <f>Demographic!C4</f>
         <v>0</v>
       </c>
       <c r="F4" s="29" t="s">
@@ -18771,23 +18771,23 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="50" t="s">
         <v>874</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="48" t="s">
         <v>877</v>
       </c>
-      <c r="E6" s="47"/>
+      <c r="E6" s="48"/>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18797,8 +18797,8 @@
       <c r="C8" s="11" t="s">
         <v>875</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18808,38 +18808,38 @@
       <c r="C9" s="11" t="s">
         <v>876</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
       <c r="L9" s="9"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="48" t="s">
         <v>873</v>
       </c>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47" t="s">
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
     </row>
     <row r="12" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="17" t="s">
         <v>246</v>
       </c>
@@ -20210,7 +20210,7 @@
       <c r="M72" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1cQaOwOaKk84IX+9qLi39s08wJrqkuKsOb2YmMIGeapZETVuOIPL+AzUI9X4UjYpq3MPJDH1PMA+0hvxFM1Pww==" saltValue="POm5tfjvwNqIvoKd+cWZBQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="95izMwSDm8BO+RePBsYZRag7AgGiJlyeZtE7HH5xOFXEDORXmUm/F3JgNHyC0ze/OAbRAQiBDX8xj/2h+qZyxw==" saltValue="DV6UMWuvly0hrPZajVp6fw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="12">
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -20263,43 +20263,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="2:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>872</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3" t="e">
         <f>Demographic!V2</f>
@@ -22298,7 +22298,7 @@
       <c r="E202" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="w6UkHHyEZ3G/cv7A4EGQY4UUV5JVBOkFluPXfDRH8P+oGlsrsB3y4slxf3BKgYKSyqhi6l4OatIK2mb0R53L6A==" saltValue="Yq/UzbwNLdxXbedOMGwCrQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vMxe7EuyOzimp0vDaTqSA5+yQbA3Nos1MMPhub+PDtTCozsmrQOODaIs4HfwFTzeUb5CziWyBfGvyY9g/muZLw==" saltValue="OEWwQUp/aCGkqHzCiYlm+Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState ref="O8:P202">
     <sortCondition ref="O8"/>
   </sortState>
@@ -22339,40 +22339,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
     </row>
     <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>

</xml_diff>

<commit_message>
Fix source type totals
</commit_message>
<xml_diff>
--- a/public/templates/NHWA_Module_1.xlsx
+++ b/public/templates/NHWA_Module_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170F7B5-9FDD-48AD-AA8A-C9295F2817F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92BF665-2E91-4B98-8373-1D6686C347A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ZzPHAP2X1LEhzickjAxTwFeFsu64OF2YSV9noiGGILhhia7PwjhHof1YVZjpCJLGeWi4dVUPnFnvXCPTB91hvA==" workbookSaltValue="Qc1qE8MbNZmsa3u02F1Qfw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1331,7 +1331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6750" uniqueCount="2627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6762" uniqueCount="2627">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -9385,7 +9385,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -9514,16 +9514,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -9533,6 +9533,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -9928,25 +9934,25 @@
       <c r="A1" s="42" t="s">
         <v>991</v>
       </c>
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
       <c r="V1" s="12"/>
@@ -9966,25 +9972,25 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="13" t="e">
@@ -10152,41 +10158,41 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48" t="s">
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48" t="s">
+      <c r="I6" s="47"/>
+      <c r="J6" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48" t="s">
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48" t="s">
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47" t="s">
         <v>868</v>
       </c>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
       <c r="Y6" s="8" t="s">
         <v>160</v>
       </c>
@@ -10213,9 +10219,9 @@
       </c>
     </row>
     <row r="7" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
       <c r="E7" s="18" t="s">
         <v>45</v>
       </c>
@@ -13461,13 +13467,13 @@
       </c>
     </row>
     <row r="69" spans="2:31" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="48" t="s">
+      <c r="B69" s="47" t="s">
         <v>2626</v>
       </c>
-      <c r="C69" s="48"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
-      <c r="F69" s="48"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
       <c r="Y69" s="8" t="s">
         <v>116</v>
       </c>
@@ -13494,11 +13500,11 @@
       </c>
     </row>
     <row r="70" spans="2:31" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="49"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="49"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="48"/>
       <c r="Y70" s="8" t="s">
         <v>117</v>
       </c>
@@ -18626,11 +18632,6 @@
     <protectedRange sqref="D9:R17 Q4 D19:R23 D25:R67 D8:T8 D18:T18 D24:T24" name="Range1"/>
   </protectedRanges>
   <mergeCells count="12">
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="R6:T6"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="B2:R2"/>
     <mergeCell ref="E6:G6"/>
@@ -18638,6 +18639,11 @@
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="R6:T6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:T67" xr:uid="{AAA47058-289B-4A8A-B387-ECA3D8362AA8}">
@@ -18694,36 +18700,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
     </row>
     <row r="2" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
       <c r="N2" s="8" t="e">
         <f>Demographic!V2</f>
         <v>#N/A</v>
@@ -18771,23 +18777,23 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>874</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>877</v>
       </c>
-      <c r="E6" s="48"/>
+      <c r="E6" s="47"/>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="48"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="50"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18797,8 +18803,8 @@
       <c r="C8" s="11" t="s">
         <v>875</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18808,38 +18814,38 @@
       <c r="C9" s="11" t="s">
         <v>876</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="L9" s="9"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="47" t="s">
         <v>873</v>
       </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48" t="s">
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
     </row>
     <row r="12" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="17" t="s">
         <v>246</v>
       </c>
@@ -20263,43 +20269,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="2:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>872</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3" t="e">
         <f>Demographic!V2</f>
@@ -22318,10 +22324,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:P112"/>
+  <dimension ref="A1:AB112"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
@@ -22334,47 +22340,49 @@
     <col min="2" max="2" width="10.140625" style="22" customWidth="1"/>
     <col min="3" max="3" width="67" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="15" width="16.7109375" style="22" customWidth="1"/>
-    <col min="16" max="31" width="9.140625" style="22" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="22" customWidth="1"/>
+    <col min="17" max="28" width="9.140625" style="53" hidden="1" customWidth="1"/>
+    <col min="29" max="31" width="9.140625" style="22" customWidth="1"/>
     <col min="32" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-    </row>
-    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+    <row r="1" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="49" t="s">
         <v>258</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-    </row>
-    <row r="3" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+    </row>
+    <row r="3" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -22390,7 +22398,7 @@
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
         <v>2</v>
       </c>
@@ -22413,7 +22421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="4"/>
@@ -22429,7 +22437,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="51" t="s">
         <v>36</v>
       </c>
@@ -22451,7 +22459,7 @@
       <c r="N6" s="51"/>
       <c r="O6" s="51"/>
     </row>
-    <row r="7" spans="1:16" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
       <c r="D7" s="24" t="s">
@@ -22490,8 +22498,44 @@
       <c r="O7" s="24" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="S7" s="17" t="s">
+        <v>894</v>
+      </c>
+      <c r="T7" s="17" t="s">
+        <v>895</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="V7" s="17" t="s">
+        <v>896</v>
+      </c>
+      <c r="W7" s="17" t="s">
+        <v>897</v>
+      </c>
+      <c r="X7" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y7" s="17" t="s">
+        <v>900</v>
+      </c>
+      <c r="Z7" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA7" s="17" t="s">
+        <v>899</v>
+      </c>
+      <c r="AB7" s="17" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
         <v>259</v>
       </c>
@@ -22549,8 +22593,56 @@
         <f t="shared" si="0"/>
         <v>☐</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="45" t="b">
+        <f>IF(OR(Q$9 = TRUE, Q$10 = TRUE, Q$17 = TRUE), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="45" t="b">
+        <f t="shared" ref="R8:AB8" si="1">IF(OR(R$9 = TRUE, R$10 = TRUE, R$17 = TRUE), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>311</v>
       </c>
@@ -22597,8 +22689,56 @@
         <v>2624</v>
       </c>
       <c r="P9" s="23"/>
-    </row>
-    <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="54" t="b">
+        <f>IF(D9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="54" t="b">
+        <f>IF(E9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="54" t="b">
+        <f>IF(F9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="54" t="b">
+        <f>IF(G9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="54" t="b">
+        <f>IF(H9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="54" t="b">
+        <f>IF(I9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W9" s="54" t="b">
+        <f>IF(J9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="54" t="b">
+        <f>IF(K9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="54" t="b">
+        <f>IF(L9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="54" t="b">
+        <f>IF(M9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="54" t="b">
+        <f>IF(N9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="54" t="b">
+        <f>IF(O9 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>260</v>
       </c>
@@ -22645,8 +22785,56 @@
         <v>2624</v>
       </c>
       <c r="P10" s="23"/>
-    </row>
-    <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q10" s="54" t="b">
+        <f>IF(D10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="54" t="b">
+        <f>IF(E10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="54" t="b">
+        <f>IF(F10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="54" t="b">
+        <f>IF(G10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="54" t="b">
+        <f>IF(H10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V10" s="54" t="b">
+        <f>IF(I10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="54" t="b">
+        <f>IF(J10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="54" t="b">
+        <f>IF(K10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="54" t="b">
+        <f>IF(L10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="54" t="b">
+        <f>IF(M10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="54" t="b">
+        <f>IF(N10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="54" t="b">
+        <f>IF(O10 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>261</v>
       </c>
@@ -22693,8 +22881,56 @@
         <v>2624</v>
       </c>
       <c r="P11" s="23"/>
-    </row>
-    <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="54" t="b">
+        <f>IF(D11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="54" t="b">
+        <f>IF(E11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="54" t="b">
+        <f>IF(F11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="54" t="b">
+        <f>IF(G11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="54" t="b">
+        <f>IF(H11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="54" t="b">
+        <f>IF(I11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W11" s="54" t="b">
+        <f>IF(J11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="54" t="b">
+        <f>IF(K11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="54" t="b">
+        <f>IF(L11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="54" t="b">
+        <f>IF(M11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="54" t="b">
+        <f>IF(N11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="54" t="b">
+        <f>IF(O11 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
         <v>262</v>
       </c>
@@ -22741,8 +22977,56 @@
         <v>2624</v>
       </c>
       <c r="P12" s="23"/>
-    </row>
-    <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="54" t="b">
+        <f>IF(D12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="54" t="b">
+        <f>IF(E12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="54" t="b">
+        <f>IF(F12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="54" t="b">
+        <f>IF(G12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="54" t="b">
+        <f>IF(H12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="54" t="b">
+        <f>IF(I12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W12" s="54" t="b">
+        <f>IF(J12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X12" s="54" t="b">
+        <f>IF(K12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="54" t="b">
+        <f>IF(L12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="54" t="b">
+        <f>IF(M12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="54" t="b">
+        <f>IF(N12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="54" t="b">
+        <f>IF(O12 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>263</v>
       </c>
@@ -22789,8 +23073,56 @@
         <v>2624</v>
       </c>
       <c r="P13" s="23"/>
-    </row>
-    <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q13" s="54" t="b">
+        <f>IF(D13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="54" t="b">
+        <f>IF(E13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="54" t="b">
+        <f>IF(F13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="54" t="b">
+        <f>IF(G13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="54" t="b">
+        <f>IF(H13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="54" t="b">
+        <f>IF(I13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="54" t="b">
+        <f>IF(J13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="54" t="b">
+        <f>IF(K13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="54" t="b">
+        <f>IF(L13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="54" t="b">
+        <f>IF(M13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="54" t="b">
+        <f>IF(N13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="54" t="b">
+        <f>IF(O13 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>264</v>
       </c>
@@ -22837,8 +23169,56 @@
         <v>2624</v>
       </c>
       <c r="P14" s="23"/>
-    </row>
-    <row r="15" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="54" t="b">
+        <f>IF(D14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="54" t="b">
+        <f>IF(E14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="54" t="b">
+        <f>IF(F14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="54" t="b">
+        <f>IF(G14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="54" t="b">
+        <f>IF(H14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V14" s="54" t="b">
+        <f>IF(I14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="54" t="b">
+        <f>IF(J14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X14" s="54" t="b">
+        <f>IF(K14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="54" t="b">
+        <f>IF(L14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="54" t="b">
+        <f>IF(M14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="54" t="b">
+        <f>IF(N14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="54" t="b">
+        <f>IF(O14 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>265</v>
       </c>
@@ -22885,8 +23265,56 @@
         <v>2624</v>
       </c>
       <c r="P15" s="23"/>
-    </row>
-    <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="54" t="b">
+        <f>IF(D15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="54" t="b">
+        <f>IF(E15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="54" t="b">
+        <f>IF(F15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="54" t="b">
+        <f>IF(G15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="54" t="b">
+        <f>IF(H15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="54" t="b">
+        <f>IF(I15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W15" s="54" t="b">
+        <f>IF(J15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="54" t="b">
+        <f>IF(K15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="54" t="b">
+        <f>IF(L15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="54" t="b">
+        <f>IF(M15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="54" t="b">
+        <f>IF(N15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="54" t="b">
+        <f>IF(O15 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>266</v>
       </c>
@@ -22933,8 +23361,56 @@
         <v>2624</v>
       </c>
       <c r="P16" s="23"/>
-    </row>
-    <row r="17" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q16" s="54" t="b">
+        <f>IF(D16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="54" t="b">
+        <f>IF(E16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="54" t="b">
+        <f>IF(F16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="54" t="b">
+        <f>IF(G16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="54" t="b">
+        <f>IF(H16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="54" t="b">
+        <f>IF(I16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="54" t="b">
+        <f>IF(J16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="54" t="b">
+        <f>IF(K16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="54" t="b">
+        <f>IF(L16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="54" t="b">
+        <f>IF(M16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="54" t="b">
+        <f>IF(N16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="54" t="b">
+        <f>IF(O16 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>267</v>
       </c>
@@ -22981,8 +23457,56 @@
         <v>2624</v>
       </c>
       <c r="P17" s="23"/>
-    </row>
-    <row r="18" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="54" t="b">
+        <f>IF(D17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="54" t="b">
+        <f>IF(E17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="54" t="b">
+        <f>IF(F17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="54" t="b">
+        <f>IF(G17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="54" t="b">
+        <f>IF(H17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V17" s="54" t="b">
+        <f>IF(I17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="54" t="b">
+        <f>IF(J17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="54" t="b">
+        <f>IF(K17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="54" t="b">
+        <f>IF(L17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="54" t="b">
+        <f>IF(M17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="54" t="b">
+        <f>IF(N17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="54" t="b">
+        <f>IF(O17 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
         <v>268</v>
       </c>
@@ -22993,56 +23517,104 @@
         <v>871</v>
       </c>
       <c r="D18" s="45" t="str">
-        <f t="shared" ref="D18:O18" si="1">IF(OR(D$19 = _true, D$21 = _true, D$23 = _true), _true, _false)</f>
+        <f t="shared" ref="D18:O18" si="2">IF(OR(D$19 = _true, D$21 = _true, D$23 = _true), _true, _false)</f>
         <v>☐</v>
       </c>
       <c r="E18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="F18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="G18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="H18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="J18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="K18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="L18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="M18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="N18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="O18" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>☐</v>
       </c>
       <c r="P18" s="23"/>
-    </row>
-    <row r="19" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q18" s="45" t="b">
+        <f>IF(OR(Q$19 = TRUE, Q$21 = TRUE, Q$23 = TRUE), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="45" t="b">
+        <f t="shared" ref="R18:AB18" si="3">IF(OR(R$19 = TRUE, R$21 = TRUE, R$23 = TRUE), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>269</v>
       </c>
@@ -23089,8 +23661,56 @@
         <v>2624</v>
       </c>
       <c r="P19" s="23"/>
-    </row>
-    <row r="20" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q19" s="54" t="b">
+        <f>IF(D19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="54" t="b">
+        <f>IF(E19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="54" t="b">
+        <f>IF(F19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="54" t="b">
+        <f>IF(G19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="54" t="b">
+        <f>IF(H19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="54" t="b">
+        <f>IF(I19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W19" s="54" t="b">
+        <f>IF(J19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X19" s="54" t="b">
+        <f>IF(K19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="54" t="b">
+        <f>IF(L19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="54" t="b">
+        <f>IF(M19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="54" t="b">
+        <f>IF(N19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="54" t="b">
+        <f>IF(O19 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>270</v>
       </c>
@@ -23137,8 +23757,56 @@
         <v>2624</v>
       </c>
       <c r="P20" s="23"/>
-    </row>
-    <row r="21" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="54" t="b">
+        <f>IF(D20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="54" t="b">
+        <f>IF(E20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="54" t="b">
+        <f>IF(F20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="54" t="b">
+        <f>IF(G20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="54" t="b">
+        <f>IF(H20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V20" s="54" t="b">
+        <f>IF(I20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W20" s="54" t="b">
+        <f>IF(J20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X20" s="54" t="b">
+        <f>IF(K20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="54" t="b">
+        <f>IF(L20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="54" t="b">
+        <f>IF(M20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="54" t="b">
+        <f>IF(N20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="54" t="b">
+        <f>IF(O20 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>271</v>
       </c>
@@ -23185,8 +23853,56 @@
         <v>2624</v>
       </c>
       <c r="P21" s="23"/>
-    </row>
-    <row r="22" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="54" t="b">
+        <f>IF(D21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="54" t="b">
+        <f>IF(E21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="54" t="b">
+        <f>IF(F21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="54" t="b">
+        <f>IF(G21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="54" t="b">
+        <f>IF(H21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="54" t="b">
+        <f>IF(I21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="54" t="b">
+        <f>IF(J21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X21" s="54" t="b">
+        <f>IF(K21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="54" t="b">
+        <f>IF(L21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="54" t="b">
+        <f>IF(M21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="54" t="b">
+        <f>IF(N21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="54" t="b">
+        <f>IF(O21 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>272</v>
       </c>
@@ -23233,8 +23949,56 @@
         <v>2624</v>
       </c>
       <c r="P22" s="23"/>
-    </row>
-    <row r="23" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q22" s="54" t="b">
+        <f>IF(D22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="54" t="b">
+        <f>IF(E22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="54" t="b">
+        <f>IF(F22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="54" t="b">
+        <f>IF(G22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="54" t="b">
+        <f>IF(H22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="54" t="b">
+        <f>IF(I22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="54" t="b">
+        <f>IF(J22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="54" t="b">
+        <f>IF(K22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="54" t="b">
+        <f>IF(L22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="54" t="b">
+        <f>IF(M22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="54" t="b">
+        <f>IF(N22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="54" t="b">
+        <f>IF(O22 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>273</v>
       </c>
@@ -23281,8 +24045,56 @@
         <v>2624</v>
       </c>
       <c r="P23" s="23"/>
-    </row>
-    <row r="24" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q23" s="54" t="b">
+        <f>IF(D23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="54" t="b">
+        <f>IF(E23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="54" t="b">
+        <f>IF(F23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="54" t="b">
+        <f>IF(G23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U23" s="54" t="b">
+        <f>IF(H23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V23" s="54" t="b">
+        <f>IF(I23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W23" s="54" t="b">
+        <f>IF(J23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X23" s="54" t="b">
+        <f>IF(K23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="54" t="b">
+        <f>IF(L23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="54" t="b">
+        <f>IF(M23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="54" t="b">
+        <f>IF(N23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="54" t="b">
+        <f>IF(O23 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
         <v>274</v>
       </c>
@@ -23293,56 +24105,104 @@
         <v>6</v>
       </c>
       <c r="D24" s="45" t="str">
-        <f t="shared" ref="D24:O24" si="2">IF(OR(D$25 = _true, D$26 = _true, D$27 = _true), _true, _false)</f>
+        <f t="shared" ref="D24:O24" si="4">IF(OR(D$25 = _true, D$26 = _true, D$27 = _true), _true, _false)</f>
         <v>☐</v>
       </c>
       <c r="E24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="F24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="G24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="H24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="I24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="J24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="K24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="L24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="M24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="N24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="O24" s="45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>☐</v>
       </c>
       <c r="P24" s="23"/>
-    </row>
-    <row r="25" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q24" s="45" t="b">
+        <f>IF(OR(Q$25 = TRUE, Q$26 = TRUE, Q$27 = TRUE), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="45" t="b">
+        <f t="shared" ref="R24:AB24" si="5">IF(OR(R$25 = TRUE, R$26 = TRUE, R$27 = TRUE), TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="45" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
         <v>275</v>
       </c>
@@ -23389,8 +24249,56 @@
         <v>2624</v>
       </c>
       <c r="P25" s="23"/>
-    </row>
-    <row r="26" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q25" s="54" t="b">
+        <f>IF(D25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="54" t="b">
+        <f>IF(E25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S25" s="54" t="b">
+        <f>IF(F25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="54" t="b">
+        <f>IF(G25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U25" s="54" t="b">
+        <f>IF(H25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V25" s="54" t="b">
+        <f>IF(I25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W25" s="54" t="b">
+        <f>IF(J25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X25" s="54" t="b">
+        <f>IF(K25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="54" t="b">
+        <f>IF(L25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="54" t="b">
+        <f>IF(M25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="54" t="b">
+        <f>IF(N25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="54" t="b">
+        <f>IF(O25 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>276</v>
       </c>
@@ -23437,8 +24345,56 @@
         <v>2624</v>
       </c>
       <c r="P26" s="23"/>
-    </row>
-    <row r="27" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q26" s="54" t="b">
+        <f>IF(D26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="54" t="b">
+        <f>IF(E26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="54" t="b">
+        <f>IF(F26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T26" s="54" t="b">
+        <f>IF(G26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="54" t="b">
+        <f>IF(H26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V26" s="54" t="b">
+        <f>IF(I26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W26" s="54" t="b">
+        <f>IF(J26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X26" s="54" t="b">
+        <f>IF(K26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="54" t="b">
+        <f>IF(L26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="54" t="b">
+        <f>IF(M26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="54" t="b">
+        <f>IF(N26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="54" t="b">
+        <f>IF(O26 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>277</v>
       </c>
@@ -23485,8 +24441,56 @@
         <v>2624</v>
       </c>
       <c r="P27" s="23"/>
-    </row>
-    <row r="28" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q27" s="54" t="b">
+        <f>IF(D27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="54" t="b">
+        <f>IF(E27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="54" t="b">
+        <f>IF(F27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T27" s="54" t="b">
+        <f>IF(G27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U27" s="54" t="b">
+        <f>IF(H27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V27" s="54" t="b">
+        <f>IF(I27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W27" s="54" t="b">
+        <f>IF(J27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X27" s="54" t="b">
+        <f>IF(K27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="54" t="b">
+        <f>IF(L27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="54" t="b">
+        <f>IF(M27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="54" t="b">
+        <f>IF(N27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="54" t="b">
+        <f>IF(O27 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>278</v>
       </c>
@@ -23533,8 +24537,56 @@
         <v>2624</v>
       </c>
       <c r="P28" s="23"/>
-    </row>
-    <row r="29" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q28" s="54" t="b">
+        <f>IF(D28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="54" t="b">
+        <f>IF(E28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S28" s="54" t="b">
+        <f>IF(F28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T28" s="54" t="b">
+        <f>IF(G28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="54" t="b">
+        <f>IF(H28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V28" s="54" t="b">
+        <f>IF(I28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W28" s="54" t="b">
+        <f>IF(J28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X28" s="54" t="b">
+        <f>IF(K28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="54" t="b">
+        <f>IF(L28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="54" t="b">
+        <f>IF(M28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="54" t="b">
+        <f>IF(N28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="54" t="b">
+        <f>IF(O28 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
         <v>279</v>
       </c>
@@ -23581,8 +24633,56 @@
         <v>2624</v>
       </c>
       <c r="P29" s="23"/>
-    </row>
-    <row r="30" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q29" s="54" t="b">
+        <f>IF(D29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="54" t="b">
+        <f>IF(E29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="54" t="b">
+        <f>IF(F29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="54" t="b">
+        <f>IF(G29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U29" s="54" t="b">
+        <f>IF(H29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V29" s="54" t="b">
+        <f>IF(I29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W29" s="54" t="b">
+        <f>IF(J29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X29" s="54" t="b">
+        <f>IF(K29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="54" t="b">
+        <f>IF(L29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="54" t="b">
+        <f>IF(M29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="54" t="b">
+        <f>IF(N29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="54" t="b">
+        <f>IF(O29 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
         <v>280</v>
       </c>
@@ -23629,8 +24729,56 @@
         <v>2624</v>
       </c>
       <c r="P30" s="23"/>
-    </row>
-    <row r="31" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q30" s="54" t="b">
+        <f>IF(D30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="54" t="b">
+        <f>IF(E30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="54" t="b">
+        <f>IF(F30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T30" s="54" t="b">
+        <f>IF(G30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U30" s="54" t="b">
+        <f>IF(H30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="54" t="b">
+        <f>IF(I30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W30" s="54" t="b">
+        <f>IF(J30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X30" s="54" t="b">
+        <f>IF(K30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="54" t="b">
+        <f>IF(L30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="54" t="b">
+        <f>IF(M30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="54" t="b">
+        <f>IF(N30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="54" t="b">
+        <f>IF(O30 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
         <v>281</v>
       </c>
@@ -23677,8 +24825,56 @@
         <v>2624</v>
       </c>
       <c r="P31" s="23"/>
-    </row>
-    <row r="32" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q31" s="54" t="b">
+        <f>IF(D31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="54" t="b">
+        <f>IF(E31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="54" t="b">
+        <f>IF(F31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="54" t="b">
+        <f>IF(G31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="54" t="b">
+        <f>IF(H31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="54" t="b">
+        <f>IF(I31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W31" s="54" t="b">
+        <f>IF(J31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X31" s="54" t="b">
+        <f>IF(K31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="54" t="b">
+        <f>IF(L31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="54" t="b">
+        <f>IF(M31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="54" t="b">
+        <f>IF(N31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="54" t="b">
+        <f>IF(O31 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>282</v>
       </c>
@@ -23725,8 +24921,56 @@
         <v>2624</v>
       </c>
       <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q32" s="54" t="b">
+        <f>IF(D32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="54" t="b">
+        <f>IF(E32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="54" t="b">
+        <f>IF(F32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T32" s="54" t="b">
+        <f>IF(G32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U32" s="54" t="b">
+        <f>IF(H32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V32" s="54" t="b">
+        <f>IF(I32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W32" s="54" t="b">
+        <f>IF(J32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X32" s="54" t="b">
+        <f>IF(K32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y32" s="54" t="b">
+        <f>IF(L32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z32" s="54" t="b">
+        <f>IF(M32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA32" s="54" t="b">
+        <f>IF(N32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="54" t="b">
+        <f>IF(O32 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
         <v>283</v>
       </c>
@@ -23773,8 +25017,56 @@
         <v>2624</v>
       </c>
       <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q33" s="54" t="b">
+        <f>IF(D33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="54" t="b">
+        <f>IF(E33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S33" s="54" t="b">
+        <f>IF(F33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T33" s="54" t="b">
+        <f>IF(G33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U33" s="54" t="b">
+        <f>IF(H33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V33" s="54" t="b">
+        <f>IF(I33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W33" s="54" t="b">
+        <f>IF(J33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X33" s="54" t="b">
+        <f>IF(K33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y33" s="54" t="b">
+        <f>IF(L33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z33" s="54" t="b">
+        <f>IF(M33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA33" s="54" t="b">
+        <f>IF(N33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="54" t="b">
+        <f>IF(O33 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="37" t="s">
         <v>284</v>
       </c>
@@ -23821,8 +25113,56 @@
         <v>2624</v>
       </c>
       <c r="P34" s="23"/>
-    </row>
-    <row r="35" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q34" s="54" t="b">
+        <f>IF(D34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="54" t="b">
+        <f>IF(E34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S34" s="54" t="b">
+        <f>IF(F34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T34" s="54" t="b">
+        <f>IF(G34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U34" s="54" t="b">
+        <f>IF(H34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V34" s="54" t="b">
+        <f>IF(I34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W34" s="54" t="b">
+        <f>IF(J34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X34" s="54" t="b">
+        <f>IF(K34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y34" s="54" t="b">
+        <f>IF(L34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z34" s="54" t="b">
+        <f>IF(M34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA34" s="54" t="b">
+        <f>IF(N34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB34" s="54" t="b">
+        <f>IF(O34 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="s">
         <v>285</v>
       </c>
@@ -23869,8 +25209,56 @@
         <v>2624</v>
       </c>
       <c r="P35" s="23"/>
-    </row>
-    <row r="36" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q35" s="54" t="b">
+        <f>IF(D35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R35" s="54" t="b">
+        <f>IF(E35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S35" s="54" t="b">
+        <f>IF(F35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T35" s="54" t="b">
+        <f>IF(G35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U35" s="54" t="b">
+        <f>IF(H35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V35" s="54" t="b">
+        <f>IF(I35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W35" s="54" t="b">
+        <f>IF(J35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X35" s="54" t="b">
+        <f>IF(K35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y35" s="54" t="b">
+        <f>IF(L35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z35" s="54" t="b">
+        <f>IF(M35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA35" s="54" t="b">
+        <f>IF(N35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB35" s="54" t="b">
+        <f>IF(O35 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="s">
         <v>286</v>
       </c>
@@ -23917,8 +25305,56 @@
         <v>2624</v>
       </c>
       <c r="P36" s="23"/>
-    </row>
-    <row r="37" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q36" s="54" t="b">
+        <f>IF(D36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R36" s="54" t="b">
+        <f>IF(E36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S36" s="54" t="b">
+        <f>IF(F36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T36" s="54" t="b">
+        <f>IF(G36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U36" s="54" t="b">
+        <f>IF(H36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V36" s="54" t="b">
+        <f>IF(I36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W36" s="54" t="b">
+        <f>IF(J36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X36" s="54" t="b">
+        <f>IF(K36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="54" t="b">
+        <f>IF(L36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z36" s="54" t="b">
+        <f>IF(M36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA36" s="54" t="b">
+        <f>IF(N36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB36" s="54" t="b">
+        <f>IF(O36 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
         <v>287</v>
       </c>
@@ -23965,8 +25401,56 @@
         <v>2624</v>
       </c>
       <c r="P37" s="23"/>
-    </row>
-    <row r="38" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="54" t="b">
+        <f>IF(D37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="54" t="b">
+        <f>IF(E37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="54" t="b">
+        <f>IF(F37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="54" t="b">
+        <f>IF(G37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U37" s="54" t="b">
+        <f>IF(H37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V37" s="54" t="b">
+        <f>IF(I37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W37" s="54" t="b">
+        <f>IF(J37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X37" s="54" t="b">
+        <f>IF(K37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="54" t="b">
+        <f>IF(L37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z37" s="54" t="b">
+        <f>IF(M37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA37" s="54" t="b">
+        <f>IF(N37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB37" s="54" t="b">
+        <f>IF(O37 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="s">
         <v>288</v>
       </c>
@@ -24013,8 +25497,56 @@
         <v>2624</v>
       </c>
       <c r="P38" s="23"/>
-    </row>
-    <row r="39" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q38" s="54" t="b">
+        <f>IF(D38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="54" t="b">
+        <f>IF(E38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="54" t="b">
+        <f>IF(F38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T38" s="54" t="b">
+        <f>IF(G38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U38" s="54" t="b">
+        <f>IF(H38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V38" s="54" t="b">
+        <f>IF(I38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W38" s="54" t="b">
+        <f>IF(J38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X38" s="54" t="b">
+        <f>IF(K38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y38" s="54" t="b">
+        <f>IF(L38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z38" s="54" t="b">
+        <f>IF(M38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA38" s="54" t="b">
+        <f>IF(N38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB38" s="54" t="b">
+        <f>IF(O38 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
         <v>289</v>
       </c>
@@ -24061,8 +25593,56 @@
         <v>2624</v>
       </c>
       <c r="P39" s="23"/>
-    </row>
-    <row r="40" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q39" s="54" t="b">
+        <f>IF(D39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R39" s="54" t="b">
+        <f>IF(E39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="54" t="b">
+        <f>IF(F39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T39" s="54" t="b">
+        <f>IF(G39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U39" s="54" t="b">
+        <f>IF(H39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V39" s="54" t="b">
+        <f>IF(I39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W39" s="54" t="b">
+        <f>IF(J39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X39" s="54" t="b">
+        <f>IF(K39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="54" t="b">
+        <f>IF(L39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z39" s="54" t="b">
+        <f>IF(M39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="54" t="b">
+        <f>IF(N39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB39" s="54" t="b">
+        <f>IF(O39 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
         <v>290</v>
       </c>
@@ -24109,8 +25689,56 @@
         <v>2624</v>
       </c>
       <c r="P40" s="23"/>
-    </row>
-    <row r="41" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q40" s="54" t="b">
+        <f>IF(D40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R40" s="54" t="b">
+        <f>IF(E40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="54" t="b">
+        <f>IF(F40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="54" t="b">
+        <f>IF(G40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U40" s="54" t="b">
+        <f>IF(H40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V40" s="54" t="b">
+        <f>IF(I40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W40" s="54" t="b">
+        <f>IF(J40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X40" s="54" t="b">
+        <f>IF(K40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y40" s="54" t="b">
+        <f>IF(L40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z40" s="54" t="b">
+        <f>IF(M40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA40" s="54" t="b">
+        <f>IF(N40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB40" s="54" t="b">
+        <f>IF(O40 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
         <v>291</v>
       </c>
@@ -24157,8 +25785,56 @@
         <v>2624</v>
       </c>
       <c r="P41" s="23"/>
-    </row>
-    <row r="42" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q41" s="54" t="b">
+        <f>IF(D41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R41" s="54" t="b">
+        <f>IF(E41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S41" s="54" t="b">
+        <f>IF(F41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T41" s="54" t="b">
+        <f>IF(G41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U41" s="54" t="b">
+        <f>IF(H41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V41" s="54" t="b">
+        <f>IF(I41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W41" s="54" t="b">
+        <f>IF(J41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X41" s="54" t="b">
+        <f>IF(K41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="54" t="b">
+        <f>IF(L41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z41" s="54" t="b">
+        <f>IF(M41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA41" s="54" t="b">
+        <f>IF(N41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB41" s="54" t="b">
+        <f>IF(O41 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
         <v>292</v>
       </c>
@@ -24205,8 +25881,56 @@
         <v>2624</v>
       </c>
       <c r="P42" s="23"/>
-    </row>
-    <row r="43" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q42" s="54" t="b">
+        <f>IF(D42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R42" s="54" t="b">
+        <f>IF(E42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S42" s="54" t="b">
+        <f>IF(F42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T42" s="54" t="b">
+        <f>IF(G42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U42" s="54" t="b">
+        <f>IF(H42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V42" s="54" t="b">
+        <f>IF(I42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W42" s="54" t="b">
+        <f>IF(J42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X42" s="54" t="b">
+        <f>IF(K42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y42" s="54" t="b">
+        <f>IF(L42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z42" s="54" t="b">
+        <f>IF(M42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA42" s="54" t="b">
+        <f>IF(N42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="54" t="b">
+        <f>IF(O42 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="s">
         <v>293</v>
       </c>
@@ -24253,8 +25977,56 @@
         <v>2624</v>
       </c>
       <c r="P43" s="23"/>
-    </row>
-    <row r="44" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q43" s="54" t="b">
+        <f>IF(D43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R43" s="54" t="b">
+        <f>IF(E43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S43" s="54" t="b">
+        <f>IF(F43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T43" s="54" t="b">
+        <f>IF(G43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U43" s="54" t="b">
+        <f>IF(H43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V43" s="54" t="b">
+        <f>IF(I43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W43" s="54" t="b">
+        <f>IF(J43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X43" s="54" t="b">
+        <f>IF(K43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y43" s="54" t="b">
+        <f>IF(L43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z43" s="54" t="b">
+        <f>IF(M43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA43" s="54" t="b">
+        <f>IF(N43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB43" s="54" t="b">
+        <f>IF(O43 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="s">
         <v>294</v>
       </c>
@@ -24301,8 +26073,56 @@
         <v>2624</v>
       </c>
       <c r="P44" s="23"/>
-    </row>
-    <row r="45" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q44" s="54" t="b">
+        <f>IF(D44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R44" s="54" t="b">
+        <f>IF(E44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="54" t="b">
+        <f>IF(F44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T44" s="54" t="b">
+        <f>IF(G44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U44" s="54" t="b">
+        <f>IF(H44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V44" s="54" t="b">
+        <f>IF(I44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W44" s="54" t="b">
+        <f>IF(J44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X44" s="54" t="b">
+        <f>IF(K44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y44" s="54" t="b">
+        <f>IF(L44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z44" s="54" t="b">
+        <f>IF(M44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA44" s="54" t="b">
+        <f>IF(N44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB44" s="54" t="b">
+        <f>IF(O44 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="37" t="s">
         <v>295</v>
       </c>
@@ -24349,8 +26169,56 @@
         <v>2624</v>
       </c>
       <c r="P45" s="23"/>
-    </row>
-    <row r="46" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q45" s="54" t="b">
+        <f>IF(D45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R45" s="54" t="b">
+        <f>IF(E45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S45" s="54" t="b">
+        <f>IF(F45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T45" s="54" t="b">
+        <f>IF(G45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U45" s="54" t="b">
+        <f>IF(H45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V45" s="54" t="b">
+        <f>IF(I45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W45" s="54" t="b">
+        <f>IF(J45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X45" s="54" t="b">
+        <f>IF(K45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y45" s="54" t="b">
+        <f>IF(L45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z45" s="54" t="b">
+        <f>IF(M45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA45" s="54" t="b">
+        <f>IF(N45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB45" s="54" t="b">
+        <f>IF(O45 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="37" t="s">
         <v>296</v>
       </c>
@@ -24397,8 +26265,56 @@
         <v>2624</v>
       </c>
       <c r="P46" s="23"/>
-    </row>
-    <row r="47" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q46" s="54" t="b">
+        <f>IF(D46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R46" s="54" t="b">
+        <f>IF(E46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S46" s="54" t="b">
+        <f>IF(F46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T46" s="54" t="b">
+        <f>IF(G46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U46" s="54" t="b">
+        <f>IF(H46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V46" s="54" t="b">
+        <f>IF(I46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W46" s="54" t="b">
+        <f>IF(J46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X46" s="54" t="b">
+        <f>IF(K46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y46" s="54" t="b">
+        <f>IF(L46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z46" s="54" t="b">
+        <f>IF(M46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA46" s="54" t="b">
+        <f>IF(N46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB46" s="54" t="b">
+        <f>IF(O46 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="37" t="s">
         <v>297</v>
       </c>
@@ -24445,8 +26361,56 @@
         <v>2624</v>
       </c>
       <c r="P47" s="23"/>
-    </row>
-    <row r="48" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q47" s="54" t="b">
+        <f>IF(D47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R47" s="54" t="b">
+        <f>IF(E47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S47" s="54" t="b">
+        <f>IF(F47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T47" s="54" t="b">
+        <f>IF(G47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U47" s="54" t="b">
+        <f>IF(H47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V47" s="54" t="b">
+        <f>IF(I47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W47" s="54" t="b">
+        <f>IF(J47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X47" s="54" t="b">
+        <f>IF(K47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y47" s="54" t="b">
+        <f>IF(L47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z47" s="54" t="b">
+        <f>IF(M47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA47" s="54" t="b">
+        <f>IF(N47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB47" s="54" t="b">
+        <f>IF(O47 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
         <v>298</v>
       </c>
@@ -24493,8 +26457,56 @@
         <v>2624</v>
       </c>
       <c r="P48" s="23"/>
-    </row>
-    <row r="49" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q48" s="54" t="b">
+        <f>IF(D48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R48" s="54" t="b">
+        <f>IF(E48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S48" s="54" t="b">
+        <f>IF(F48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T48" s="54" t="b">
+        <f>IF(G48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U48" s="54" t="b">
+        <f>IF(H48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V48" s="54" t="b">
+        <f>IF(I48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W48" s="54" t="b">
+        <f>IF(J48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X48" s="54" t="b">
+        <f>IF(K48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y48" s="54" t="b">
+        <f>IF(L48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z48" s="54" t="b">
+        <f>IF(M48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA48" s="54" t="b">
+        <f>IF(N48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB48" s="54" t="b">
+        <f>IF(O48 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="s">
         <v>299</v>
       </c>
@@ -24541,8 +26553,56 @@
         <v>2624</v>
       </c>
       <c r="P49" s="23"/>
-    </row>
-    <row r="50" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q49" s="54" t="b">
+        <f>IF(D49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R49" s="54" t="b">
+        <f>IF(E49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S49" s="54" t="b">
+        <f>IF(F49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T49" s="54" t="b">
+        <f>IF(G49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U49" s="54" t="b">
+        <f>IF(H49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V49" s="54" t="b">
+        <f>IF(I49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W49" s="54" t="b">
+        <f>IF(J49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X49" s="54" t="b">
+        <f>IF(K49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y49" s="54" t="b">
+        <f>IF(L49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z49" s="54" t="b">
+        <f>IF(M49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA49" s="54" t="b">
+        <f>IF(N49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB49" s="54" t="b">
+        <f>IF(O49 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="37" t="s">
         <v>300</v>
       </c>
@@ -24589,8 +26649,56 @@
         <v>2624</v>
       </c>
       <c r="P50" s="23"/>
-    </row>
-    <row r="51" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q50" s="54" t="b">
+        <f>IF(D50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R50" s="54" t="b">
+        <f>IF(E50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S50" s="54" t="b">
+        <f>IF(F50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T50" s="54" t="b">
+        <f>IF(G50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U50" s="54" t="b">
+        <f>IF(H50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V50" s="54" t="b">
+        <f>IF(I50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W50" s="54" t="b">
+        <f>IF(J50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X50" s="54" t="b">
+        <f>IF(K50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y50" s="54" t="b">
+        <f>IF(L50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z50" s="54" t="b">
+        <f>IF(M50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA50" s="54" t="b">
+        <f>IF(N50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB50" s="54" t="b">
+        <f>IF(O50 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37" t="s">
         <v>301</v>
       </c>
@@ -24637,8 +26745,56 @@
         <v>2624</v>
       </c>
       <c r="P51" s="23"/>
-    </row>
-    <row r="52" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q51" s="54" t="b">
+        <f>IF(D51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R51" s="54" t="b">
+        <f>IF(E51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S51" s="54" t="b">
+        <f>IF(F51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T51" s="54" t="b">
+        <f>IF(G51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U51" s="54" t="b">
+        <f>IF(H51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V51" s="54" t="b">
+        <f>IF(I51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W51" s="54" t="b">
+        <f>IF(J51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X51" s="54" t="b">
+        <f>IF(K51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y51" s="54" t="b">
+        <f>IF(L51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z51" s="54" t="b">
+        <f>IF(M51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA51" s="54" t="b">
+        <f>IF(N51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB51" s="54" t="b">
+        <f>IF(O51 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="37" t="s">
         <v>302</v>
       </c>
@@ -24685,8 +26841,56 @@
         <v>2624</v>
       </c>
       <c r="P52" s="23"/>
-    </row>
-    <row r="53" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q52" s="54" t="b">
+        <f>IF(D52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R52" s="54" t="b">
+        <f>IF(E52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S52" s="54" t="b">
+        <f>IF(F52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T52" s="54" t="b">
+        <f>IF(G52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U52" s="54" t="b">
+        <f>IF(H52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V52" s="54" t="b">
+        <f>IF(I52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W52" s="54" t="b">
+        <f>IF(J52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X52" s="54" t="b">
+        <f>IF(K52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y52" s="54" t="b">
+        <f>IF(L52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z52" s="54" t="b">
+        <f>IF(M52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA52" s="54" t="b">
+        <f>IF(N52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB52" s="54" t="b">
+        <f>IF(O52 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="37" t="s">
         <v>303</v>
       </c>
@@ -24733,8 +26937,56 @@
         <v>2624</v>
       </c>
       <c r="P53" s="23"/>
-    </row>
-    <row r="54" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q53" s="54" t="b">
+        <f>IF(D53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R53" s="54" t="b">
+        <f>IF(E53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S53" s="54" t="b">
+        <f>IF(F53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T53" s="54" t="b">
+        <f>IF(G53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U53" s="54" t="b">
+        <f>IF(H53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V53" s="54" t="b">
+        <f>IF(I53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W53" s="54" t="b">
+        <f>IF(J53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X53" s="54" t="b">
+        <f>IF(K53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y53" s="54" t="b">
+        <f>IF(L53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z53" s="54" t="b">
+        <f>IF(M53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA53" s="54" t="b">
+        <f>IF(N53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB53" s="54" t="b">
+        <f>IF(O53 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="37" t="s">
         <v>304</v>
       </c>
@@ -24781,8 +27033,56 @@
         <v>2624</v>
       </c>
       <c r="P54" s="23"/>
-    </row>
-    <row r="55" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q54" s="54" t="b">
+        <f>IF(D54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R54" s="54" t="b">
+        <f>IF(E54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S54" s="54" t="b">
+        <f>IF(F54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T54" s="54" t="b">
+        <f>IF(G54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U54" s="54" t="b">
+        <f>IF(H54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V54" s="54" t="b">
+        <f>IF(I54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W54" s="54" t="b">
+        <f>IF(J54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X54" s="54" t="b">
+        <f>IF(K54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y54" s="54" t="b">
+        <f>IF(L54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z54" s="54" t="b">
+        <f>IF(M54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA54" s="54" t="b">
+        <f>IF(N54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB54" s="54" t="b">
+        <f>IF(O54 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="37"/>
       <c r="B55" s="25">
         <v>27</v>
@@ -24827,8 +27127,56 @@
         <v>2624</v>
       </c>
       <c r="P55" s="23"/>
-    </row>
-    <row r="56" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q55" s="54" t="b">
+        <f>IF(D55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R55" s="54" t="b">
+        <f>IF(E55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S55" s="54" t="b">
+        <f>IF(F55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T55" s="54" t="b">
+        <f>IF(G55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U55" s="54" t="b">
+        <f>IF(H55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V55" s="54" t="b">
+        <f>IF(I55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W55" s="54" t="b">
+        <f>IF(J55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X55" s="54" t="b">
+        <f>IF(K55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y55" s="54" t="b">
+        <f>IF(L55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z55" s="54" t="b">
+        <f>IF(M55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA55" s="54" t="b">
+        <f>IF(N55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB55" s="54" t="b">
+        <f>IF(O55 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="37"/>
       <c r="B56" s="25">
         <v>28</v>
@@ -24873,8 +27221,56 @@
         <v>2624</v>
       </c>
       <c r="P56" s="23"/>
-    </row>
-    <row r="57" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q56" s="54" t="b">
+        <f>IF(D56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R56" s="54" t="b">
+        <f>IF(E56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S56" s="54" t="b">
+        <f>IF(F56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T56" s="54" t="b">
+        <f>IF(G56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U56" s="54" t="b">
+        <f>IF(H56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V56" s="54" t="b">
+        <f>IF(I56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W56" s="54" t="b">
+        <f>IF(J56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X56" s="54" t="b">
+        <f>IF(K56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y56" s="54" t="b">
+        <f>IF(L56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z56" s="54" t="b">
+        <f>IF(M56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA56" s="54" t="b">
+        <f>IF(N56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB56" s="54" t="b">
+        <f>IF(O56 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="37"/>
       <c r="B57" s="25">
         <v>29</v>
@@ -24919,8 +27315,56 @@
         <v>2624</v>
       </c>
       <c r="P57" s="23"/>
-    </row>
-    <row r="58" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q57" s="54" t="b">
+        <f>IF(D57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R57" s="54" t="b">
+        <f>IF(E57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S57" s="54" t="b">
+        <f>IF(F57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T57" s="54" t="b">
+        <f>IF(G57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U57" s="54" t="b">
+        <f>IF(H57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V57" s="54" t="b">
+        <f>IF(I57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W57" s="54" t="b">
+        <f>IF(J57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X57" s="54" t="b">
+        <f>IF(K57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y57" s="54" t="b">
+        <f>IF(L57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z57" s="54" t="b">
+        <f>IF(M57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA57" s="54" t="b">
+        <f>IF(N57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB57" s="54" t="b">
+        <f>IF(O57 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="37"/>
       <c r="B58" s="25">
         <v>30</v>
@@ -24965,8 +27409,56 @@
         <v>2624</v>
       </c>
       <c r="P58" s="23"/>
-    </row>
-    <row r="59" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q58" s="54" t="b">
+        <f>IF(D58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R58" s="54" t="b">
+        <f>IF(E58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S58" s="54" t="b">
+        <f>IF(F58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T58" s="54" t="b">
+        <f>IF(G58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U58" s="54" t="b">
+        <f>IF(H58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V58" s="54" t="b">
+        <f>IF(I58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W58" s="54" t="b">
+        <f>IF(J58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X58" s="54" t="b">
+        <f>IF(K58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y58" s="54" t="b">
+        <f>IF(L58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z58" s="54" t="b">
+        <f>IF(M58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA58" s="54" t="b">
+        <f>IF(N58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB58" s="54" t="b">
+        <f>IF(O58 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="37"/>
       <c r="B59" s="25">
         <v>31</v>
@@ -25011,8 +27503,56 @@
         <v>2624</v>
       </c>
       <c r="P59" s="23"/>
-    </row>
-    <row r="60" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q59" s="54" t="b">
+        <f>IF(D59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R59" s="54" t="b">
+        <f>IF(E59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S59" s="54" t="b">
+        <f>IF(F59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T59" s="54" t="b">
+        <f>IF(G59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U59" s="54" t="b">
+        <f>IF(H59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V59" s="54" t="b">
+        <f>IF(I59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W59" s="54" t="b">
+        <f>IF(J59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X59" s="54" t="b">
+        <f>IF(K59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y59" s="54" t="b">
+        <f>IF(L59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z59" s="54" t="b">
+        <f>IF(M59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA59" s="54" t="b">
+        <f>IF(N59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB59" s="54" t="b">
+        <f>IF(O59 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="37"/>
       <c r="B60" s="25">
         <v>32</v>
@@ -25057,8 +27597,56 @@
         <v>2624</v>
       </c>
       <c r="P60" s="23"/>
-    </row>
-    <row r="61" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q60" s="54" t="b">
+        <f>IF(D60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R60" s="54" t="b">
+        <f>IF(E60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S60" s="54" t="b">
+        <f>IF(F60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T60" s="54" t="b">
+        <f>IF(G60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U60" s="54" t="b">
+        <f>IF(H60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V60" s="54" t="b">
+        <f>IF(I60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W60" s="54" t="b">
+        <f>IF(J60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X60" s="54" t="b">
+        <f>IF(K60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y60" s="54" t="b">
+        <f>IF(L60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z60" s="54" t="b">
+        <f>IF(M60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA60" s="54" t="b">
+        <f>IF(N60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB60" s="54" t="b">
+        <f>IF(O60 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="37"/>
       <c r="B61" s="25">
         <v>33</v>
@@ -25103,8 +27691,56 @@
         <v>2624</v>
       </c>
       <c r="P61" s="23"/>
-    </row>
-    <row r="62" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q61" s="54" t="b">
+        <f>IF(D61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R61" s="54" t="b">
+        <f>IF(E61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S61" s="54" t="b">
+        <f>IF(F61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T61" s="54" t="b">
+        <f>IF(G61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U61" s="54" t="b">
+        <f>IF(H61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V61" s="54" t="b">
+        <f>IF(I61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W61" s="54" t="b">
+        <f>IF(J61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X61" s="54" t="b">
+        <f>IF(K61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="54" t="b">
+        <f>IF(L61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z61" s="54" t="b">
+        <f>IF(M61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA61" s="54" t="b">
+        <f>IF(N61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB61" s="54" t="b">
+        <f>IF(O61 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37" t="s">
         <v>305</v>
       </c>
@@ -25151,8 +27787,56 @@
         <v>2624</v>
       </c>
       <c r="P62" s="23"/>
-    </row>
-    <row r="63" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q62" s="54" t="b">
+        <f>IF(D62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R62" s="54" t="b">
+        <f>IF(E62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S62" s="54" t="b">
+        <f>IF(F62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T62" s="54" t="b">
+        <f>IF(G62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U62" s="54" t="b">
+        <f>IF(H62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V62" s="54" t="b">
+        <f>IF(I62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W62" s="54" t="b">
+        <f>IF(J62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X62" s="54" t="b">
+        <f>IF(K62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y62" s="54" t="b">
+        <f>IF(L62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z62" s="54" t="b">
+        <f>IF(M62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA62" s="54" t="b">
+        <f>IF(N62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB62" s="54" t="b">
+        <f>IF(O62 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37" t="s">
         <v>306</v>
       </c>
@@ -25199,8 +27883,56 @@
         <v>2624</v>
       </c>
       <c r="P63" s="23"/>
-    </row>
-    <row r="64" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q63" s="54" t="b">
+        <f>IF(D63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R63" s="54" t="b">
+        <f>IF(E63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S63" s="54" t="b">
+        <f>IF(F63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T63" s="54" t="b">
+        <f>IF(G63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U63" s="54" t="b">
+        <f>IF(H63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V63" s="54" t="b">
+        <f>IF(I63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W63" s="54" t="b">
+        <f>IF(J63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X63" s="54" t="b">
+        <f>IF(K63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y63" s="54" t="b">
+        <f>IF(L63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z63" s="54" t="b">
+        <f>IF(M63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA63" s="54" t="b">
+        <f>IF(N63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB63" s="54" t="b">
+        <f>IF(O63 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="37" t="s">
         <v>307</v>
       </c>
@@ -25247,8 +27979,56 @@
         <v>2624</v>
       </c>
       <c r="P64" s="23"/>
-    </row>
-    <row r="65" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q64" s="54" t="b">
+        <f>IF(D64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R64" s="54" t="b">
+        <f>IF(E64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S64" s="54" t="b">
+        <f>IF(F64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T64" s="54" t="b">
+        <f>IF(G64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U64" s="54" t="b">
+        <f>IF(H64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V64" s="54" t="b">
+        <f>IF(I64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W64" s="54" t="b">
+        <f>IF(J64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X64" s="54" t="b">
+        <f>IF(K64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y64" s="54" t="b">
+        <f>IF(L64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z64" s="54" t="b">
+        <f>IF(M64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA64" s="54" t="b">
+        <f>IF(N64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB64" s="54" t="b">
+        <f>IF(O64 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37" t="s">
         <v>308</v>
       </c>
@@ -25295,8 +28075,56 @@
         <v>2624</v>
       </c>
       <c r="P65" s="23"/>
-    </row>
-    <row r="66" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q65" s="54" t="b">
+        <f>IF(D65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R65" s="54" t="b">
+        <f>IF(E65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S65" s="54" t="b">
+        <f>IF(F65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T65" s="54" t="b">
+        <f>IF(G65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U65" s="54" t="b">
+        <f>IF(H65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V65" s="54" t="b">
+        <f>IF(I65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W65" s="54" t="b">
+        <f>IF(J65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X65" s="54" t="b">
+        <f>IF(K65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y65" s="54" t="b">
+        <f>IF(L65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z65" s="54" t="b">
+        <f>IF(M65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA65" s="54" t="b">
+        <f>IF(N65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB65" s="54" t="b">
+        <f>IF(O65 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37" t="s">
         <v>309</v>
       </c>
@@ -25343,8 +28171,56 @@
         <v>2624</v>
       </c>
       <c r="P66" s="23"/>
-    </row>
-    <row r="67" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q66" s="54" t="b">
+        <f>IF(D66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R66" s="54" t="b">
+        <f>IF(E66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S66" s="54" t="b">
+        <f>IF(F66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T66" s="54" t="b">
+        <f>IF(G66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U66" s="54" t="b">
+        <f>IF(H66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V66" s="54" t="b">
+        <f>IF(I66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W66" s="54" t="b">
+        <f>IF(J66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X66" s="54" t="b">
+        <f>IF(K66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y66" s="54" t="b">
+        <f>IF(L66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z66" s="54" t="b">
+        <f>IF(M66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA66" s="54" t="b">
+        <f>IF(N66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB66" s="54" t="b">
+        <f>IF(O66 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37" t="s">
         <v>310</v>
       </c>
@@ -25391,20 +28267,68 @@
         <v>2624</v>
       </c>
       <c r="P67" s="23"/>
-    </row>
-    <row r="68" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="Q67" s="54" t="b">
+        <f>IF(D67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R67" s="54" t="b">
+        <f>IF(E67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="S67" s="54" t="b">
+        <f>IF(F67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="T67" s="54" t="b">
+        <f>IF(G67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U67" s="54" t="b">
+        <f>IF(H67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="54" t="b">
+        <f>IF(I67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="W67" s="54" t="b">
+        <f>IF(J67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="X67" s="54" t="b">
+        <f>IF(K67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y67" s="54" t="b">
+        <f>IF(L67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z67" s="54" t="b">
+        <f>IF(M67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AA67" s="54" t="b">
+        <f>IF(N67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AB67" s="54" t="b">
+        <f>IF(O67 = _true, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25438,7 +28362,7 @@
     <row r="111" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="112" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uCtvd3UxMNxQKd93hvePIxr6Vks867Ws2p+AyJIlIMe4RkeIC0snv8xSElToYqVa3kkKLDHB4i3Afbq/LSlqrQ==" saltValue="/cPtfZejiGbWGahkvZBR+w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="KZR1Xx+sEj3oVD3l7DJh8/SnXEpPGo5hzIC4CFFegizdlXGAviVTYKowUi7rNmarCQTkNQZPtHhu9oJ7l9uJoQ==" saltValue="seVRa94naZnf8LMhCHvbgw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:O2"/>
@@ -25448,6 +28372,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="Q18:AB18 Q24:AB24" formula="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>